<commit_message>
sql table relationships are established
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gigalskiy\IdeaProjects\ParsingAuto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gigalskiy\IdeaProjects\repairtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B06F13C-832D-4EA7-B0FF-2FE98C873EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F554322-D2CA-4ED4-A4CF-7EA70B0BACFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="118">
   <si>
     <t>FORD / ESCORT ('81) / 1,3 / JGA 43 kW (58 л.с.) 4800 об/мин (N) (S) (SF) 1984-1985</t>
   </si>
@@ -337,6 +337,48 @@
   </si>
   <si>
     <t>SKODA / OCTAVIA II (1Z3/1Z5)  (04-13) / 1,4 / BCA 55 kW (75 л.с.) 5000 об/мин R-Cat 2004-2009</t>
+  </si>
+  <si>
+    <t>Двигатель</t>
+  </si>
+  <si>
+    <t>Тормоза</t>
+  </si>
+  <si>
+    <t>Трансмиссия</t>
+  </si>
+  <si>
+    <t>Замена масла</t>
+  </si>
+  <si>
+    <t>Замена воздушного фильтра</t>
+  </si>
+  <si>
+    <t>Замена ГБЦ</t>
+  </si>
+  <si>
+    <t>Замена впусконого коллектора</t>
+  </si>
+  <si>
+    <t>Замена масла АКПП</t>
+  </si>
+  <si>
+    <t>Замена АКПП</t>
+  </si>
+  <si>
+    <t>Замена сальника АКПП</t>
+  </si>
+  <si>
+    <t>Замена редуктора задней оси</t>
+  </si>
+  <si>
+    <t>Замена тормозных колодок перед</t>
+  </si>
+  <si>
+    <t>Замена тормозных колодок задн</t>
+  </si>
+  <si>
+    <t>Замена тормозной жидкости</t>
   </si>
 </sst>
 </file>
@@ -399,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -410,6 +452,13 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -690,15 +739,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49" customWidth="1"/>
+    <col min="2" max="2" width="63.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -708,1756 +760,2046 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3">
-        <v>294</v>
-      </c>
-      <c r="D1" s="3">
-        <v>33</v>
-      </c>
-      <c r="E1" s="3">
-        <v>136</v>
+      <c r="C1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="4">
+        <v>0.4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1054</v>
+        <v>3306</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>339</v>
-      </c>
-      <c r="D2" s="3">
-        <v>41</v>
-      </c>
-      <c r="E2" s="3">
-        <v>193</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1561</v>
+        <v>3306</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3">
-        <v>391</v>
-      </c>
-      <c r="D3" s="3">
-        <v>40</v>
-      </c>
-      <c r="E3" s="3">
-        <v>175</v>
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1953</v>
+        <v>3306</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3">
-        <v>360</v>
-      </c>
-      <c r="D4" s="3">
-        <v>40</v>
-      </c>
-      <c r="E4" s="3">
-        <v>175</v>
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1954</v>
+        <v>3306</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3">
-        <v>393</v>
-      </c>
-      <c r="D5" s="3">
-        <v>40</v>
-      </c>
-      <c r="E5" s="3">
-        <v>175</v>
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1955</v>
+        <v>3306</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3">
-        <v>480</v>
-      </c>
-      <c r="D6" s="3">
-        <v>40</v>
-      </c>
-      <c r="E6" s="3">
-        <v>159</v>
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1956</v>
+        <v>3306</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3">
-        <v>370</v>
-      </c>
-      <c r="D7" s="3">
-        <v>40</v>
-      </c>
-      <c r="E7" s="3">
-        <v>176</v>
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="4">
+        <v>3.2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1957</v>
+        <v>3306</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3">
-        <v>352</v>
-      </c>
-      <c r="D8" s="3">
-        <v>41</v>
-      </c>
-      <c r="E8" s="3">
-        <v>127</v>
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1958</v>
+        <v>3306</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3">
-        <v>361</v>
-      </c>
-      <c r="D9" s="3">
-        <v>41</v>
-      </c>
-      <c r="E9" s="3">
-        <v>127</v>
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>2078</v>
+        <v>3306</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3">
-        <v>34</v>
-      </c>
-      <c r="D10" s="3">
-        <v>34</v>
-      </c>
-      <c r="E10" s="3">
-        <v>151</v>
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.2</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2079</v>
+        <v>3306</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3">
-        <v>81</v>
-      </c>
-      <c r="D11" s="3">
-        <v>35</v>
-      </c>
-      <c r="E11" s="3">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2080</v>
+        <v>1054</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3">
-        <v>81</v>
-      </c>
-      <c r="D12" s="3">
-        <v>35</v>
-      </c>
-      <c r="E12" s="3">
-        <v>166</v>
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2081</v>
+        <v>1054</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3">
-        <v>34</v>
-      </c>
-      <c r="D13" s="3">
-        <v>34</v>
-      </c>
-      <c r="E13" s="3">
-        <v>162</v>
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2082</v>
+        <v>1054</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3">
-        <v>34</v>
-      </c>
-      <c r="D14" s="3">
-        <v>34</v>
-      </c>
-      <c r="E14" s="3">
-        <v>162</v>
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="4">
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2083</v>
+        <v>1054</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3">
-        <v>79</v>
-      </c>
-      <c r="D15" s="3">
-        <v>36</v>
-      </c>
-      <c r="E15" s="3">
-        <v>215</v>
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2.4</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2313</v>
+        <v>1054</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="3">
-        <v>336</v>
-      </c>
-      <c r="D16" s="3">
-        <v>38</v>
-      </c>
-      <c r="E16" s="3">
-        <v>144</v>
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.7</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>2314</v>
+        <v>1054</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3">
-        <v>495</v>
-      </c>
-      <c r="D17" s="3">
-        <v>40</v>
-      </c>
-      <c r="E17" s="3">
-        <v>195</v>
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="4">
+        <v>45384</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>2315</v>
+        <v>1054</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="3">
-        <v>378</v>
-      </c>
-      <c r="D18" s="3">
-        <v>40</v>
-      </c>
-      <c r="E18" s="3">
-        <v>194</v>
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>2316</v>
+        <v>1054</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="3">
-        <v>378</v>
-      </c>
-      <c r="D19" s="3">
-        <v>40</v>
-      </c>
-      <c r="E19" s="3">
-        <v>191</v>
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="4">
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>2317</v>
+        <v>1561</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="D20" s="3">
-        <v>39</v>
-      </c>
-      <c r="E20" s="3">
-        <v>151</v>
+        <v>40</v>
+      </c>
+      <c r="E20" s="4">
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>2318</v>
+        <v>1953</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C21" s="3">
-        <v>38</v>
+        <v>360</v>
       </c>
       <c r="D21" s="3">
-        <v>38</v>
-      </c>
-      <c r="E21" s="3">
-        <v>196</v>
+        <v>40</v>
+      </c>
+      <c r="E21" s="4">
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>2319</v>
+        <v>1954</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C22" s="3">
-        <v>349</v>
+        <v>393</v>
       </c>
       <c r="D22" s="3">
-        <v>39</v>
-      </c>
-      <c r="E22" s="3">
-        <v>195</v>
+        <v>40</v>
+      </c>
+      <c r="E22" s="4">
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>2320</v>
+        <v>1955</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C23" s="3">
-        <v>349</v>
+        <v>480</v>
       </c>
       <c r="D23" s="3">
-        <v>39</v>
-      </c>
-      <c r="E23" s="3">
-        <v>195</v>
+        <v>40</v>
+      </c>
+      <c r="E23" s="4">
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>2321</v>
+        <v>1956</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C24" s="3">
-        <v>349</v>
+        <v>370</v>
       </c>
       <c r="D24" s="3">
-        <v>39</v>
-      </c>
-      <c r="E24" s="3">
-        <v>195</v>
+        <v>40</v>
+      </c>
+      <c r="E24" s="4">
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>2322</v>
+        <v>1957</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C25" s="3">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="D25" s="3">
-        <v>39</v>
-      </c>
-      <c r="E25" s="3">
-        <v>206</v>
+        <v>41</v>
+      </c>
+      <c r="E25" s="4">
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>2323</v>
+        <v>1958</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C26" s="3">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="D26" s="3">
-        <v>37</v>
-      </c>
-      <c r="E26" s="3">
-        <v>146</v>
+        <v>41</v>
+      </c>
+      <c r="E26" s="4">
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>2324</v>
+        <v>2078</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C27" s="3">
-        <v>353</v>
+        <v>34</v>
       </c>
       <c r="D27" s="3">
-        <v>37</v>
-      </c>
-      <c r="E27" s="3">
-        <v>146</v>
+        <v>34</v>
+      </c>
+      <c r="E27" s="4">
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>2325</v>
+        <v>2079</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C28" s="3">
-        <v>350</v>
+        <v>81</v>
       </c>
       <c r="D28" s="3">
-        <v>37</v>
-      </c>
-      <c r="E28" s="3">
-        <v>147</v>
+        <v>35</v>
+      </c>
+      <c r="E28" s="4">
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>2896</v>
+        <v>2080</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C29" s="3">
-        <v>361</v>
+        <v>81</v>
       </c>
       <c r="D29" s="3">
-        <v>39</v>
-      </c>
-      <c r="E29" s="3">
-        <v>133</v>
+        <v>35</v>
+      </c>
+      <c r="E29" s="4">
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>2897</v>
+        <v>2081</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C30" s="3">
-        <v>377</v>
+        <v>34</v>
       </c>
       <c r="D30" s="3">
-        <v>40</v>
-      </c>
-      <c r="E30" s="3">
+        <v>34</v>
+      </c>
+      <c r="E30" s="4">
         <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>2898</v>
+        <v>2082</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C31" s="3">
-        <v>368</v>
+        <v>34</v>
       </c>
       <c r="D31" s="3">
-        <v>41</v>
-      </c>
-      <c r="E31" s="3">
-        <v>155</v>
+        <v>34</v>
+      </c>
+      <c r="E31" s="4">
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>2899</v>
+        <v>2083</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C32" s="3">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="D32" s="3">
-        <v>22</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="E32" s="4">
+        <v>215</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>2900</v>
+        <v>2313</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C33" s="3">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D33" s="3">
-        <v>39</v>
-      </c>
-      <c r="E33" s="3">
-        <v>147</v>
+        <v>38</v>
+      </c>
+      <c r="E33" s="4">
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>2901</v>
+        <v>2314</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C34" s="3">
-        <v>384</v>
+        <v>495</v>
       </c>
       <c r="D34" s="3">
-        <v>39</v>
-      </c>
-      <c r="E34" s="3">
-        <v>149</v>
+        <v>40</v>
+      </c>
+      <c r="E34" s="4">
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>2902</v>
+        <v>2315</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C35" s="3">
-        <v>348</v>
+        <v>378</v>
       </c>
       <c r="D35" s="3">
-        <v>38</v>
-      </c>
-      <c r="E35" s="3">
-        <v>149</v>
+        <v>40</v>
+      </c>
+      <c r="E35" s="4">
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>3370</v>
+        <v>2316</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C36" s="3">
-        <v>453</v>
+        <v>378</v>
       </c>
       <c r="D36" s="3">
-        <v>42</v>
-      </c>
-      <c r="E36" s="3">
-        <v>150</v>
+        <v>40</v>
+      </c>
+      <c r="E36" s="4">
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>3371</v>
+        <v>2317</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C37" s="3">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="D37" s="3">
-        <v>42</v>
-      </c>
-      <c r="E37" s="3">
+        <v>39</v>
+      </c>
+      <c r="E37" s="4">
         <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>3372</v>
+        <v>2318</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C38" s="3">
-        <v>420</v>
+        <v>38</v>
       </c>
       <c r="D38" s="3">
-        <v>41</v>
-      </c>
-      <c r="E38" s="3">
-        <v>164</v>
+        <v>38</v>
+      </c>
+      <c r="E38" s="4">
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>3373</v>
+        <v>2319</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C39" s="3">
-        <v>452</v>
+        <v>349</v>
       </c>
       <c r="D39" s="3">
-        <v>41</v>
-      </c>
-      <c r="E39" s="3">
-        <v>161</v>
+        <v>39</v>
+      </c>
+      <c r="E39" s="4">
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>3374</v>
+        <v>2320</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C40" s="3">
-        <v>288</v>
+        <v>349</v>
       </c>
       <c r="D40" s="3">
         <v>39</v>
       </c>
-      <c r="E40" s="3">
-        <v>132</v>
+      <c r="E40" s="4">
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>3375</v>
+        <v>2321</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C41" s="3">
-        <v>256</v>
+        <v>349</v>
       </c>
       <c r="D41" s="3">
         <v>39</v>
       </c>
-      <c r="E41" s="3">
-        <v>129</v>
+      <c r="E41" s="4">
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>3376</v>
+        <v>2322</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C42" s="3">
-        <v>246</v>
+        <v>326</v>
       </c>
       <c r="D42" s="3">
         <v>39</v>
       </c>
-      <c r="E42" s="3">
-        <v>132</v>
+      <c r="E42" s="4">
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>3377</v>
+        <v>2323</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C43" s="3">
-        <v>256</v>
+        <v>353</v>
       </c>
       <c r="D43" s="3">
-        <v>39</v>
-      </c>
-      <c r="E43" s="3">
-        <v>135</v>
+        <v>37</v>
+      </c>
+      <c r="E43" s="4">
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>3378</v>
+        <v>2324</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C44" s="3">
-        <v>245</v>
+        <v>353</v>
       </c>
       <c r="D44" s="3">
         <v>37</v>
       </c>
-      <c r="E44" s="3">
-        <v>125</v>
+      <c r="E44" s="4">
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>3379</v>
+        <v>2325</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C45" s="3">
-        <v>245</v>
+        <v>350</v>
       </c>
       <c r="D45" s="3">
         <v>37</v>
       </c>
-      <c r="E45" s="3">
-        <v>125</v>
+      <c r="E45" s="4">
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>3380</v>
+        <v>2896</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C46" s="3">
-        <v>245</v>
+        <v>361</v>
       </c>
       <c r="D46" s="3">
-        <v>37</v>
-      </c>
-      <c r="E46" s="3">
-        <v>132</v>
+        <v>39</v>
+      </c>
+      <c r="E46" s="4">
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>3718</v>
+        <v>2897</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C47" s="3">
-        <v>329</v>
+        <v>377</v>
       </c>
       <c r="D47" s="3">
-        <v>35</v>
-      </c>
-      <c r="E47" s="3">
-        <v>117</v>
+        <v>40</v>
+      </c>
+      <c r="E47" s="4">
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>3719</v>
+        <v>2898</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C48" s="3">
-        <v>329</v>
+        <v>368</v>
       </c>
       <c r="D48" s="3">
-        <v>35</v>
-      </c>
-      <c r="E48" s="3">
-        <v>112</v>
+        <v>41</v>
+      </c>
+      <c r="E48" s="4">
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>3720</v>
+        <v>2899</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C49" s="3">
-        <v>329</v>
+        <v>22</v>
       </c>
       <c r="D49" s="3">
-        <v>35</v>
-      </c>
-      <c r="E49" s="3">
-        <v>112</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>3721</v>
+        <v>2900</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C50" s="3">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="D50" s="3">
-        <v>35</v>
-      </c>
-      <c r="E50" s="3">
-        <v>112</v>
+        <v>39</v>
+      </c>
+      <c r="E50" s="4">
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>3722</v>
+        <v>2901</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C51" s="3">
-        <v>330</v>
+        <v>384</v>
       </c>
       <c r="D51" s="3">
-        <v>35</v>
-      </c>
-      <c r="E51" s="3">
-        <v>111</v>
+        <v>39</v>
+      </c>
+      <c r="E51" s="4">
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>3723</v>
+        <v>2902</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C52" s="3">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="D52" s="3">
-        <v>35</v>
-      </c>
-      <c r="E52" s="3">
-        <v>112</v>
+        <v>38</v>
+      </c>
+      <c r="E52" s="4">
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>3724</v>
+        <v>3370</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C53" s="3">
-        <v>313</v>
+        <v>453</v>
       </c>
       <c r="D53" s="3">
-        <v>40</v>
-      </c>
-      <c r="E53" s="3">
-        <v>149</v>
+        <v>42</v>
+      </c>
+      <c r="E53" s="4">
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>3725</v>
+        <v>3371</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C54" s="3">
-        <v>313</v>
+        <v>453</v>
       </c>
       <c r="D54" s="3">
-        <v>40</v>
-      </c>
-      <c r="E54" s="3">
-        <v>149</v>
+        <v>42</v>
+      </c>
+      <c r="E54" s="4">
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>3726</v>
+        <v>3372</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C55" s="3">
-        <v>313</v>
+        <v>420</v>
       </c>
       <c r="D55" s="3">
-        <v>40</v>
-      </c>
-      <c r="E55" s="3">
-        <v>149</v>
+        <v>41</v>
+      </c>
+      <c r="E55" s="4">
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>3727</v>
+        <v>3373</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C56" s="3">
-        <v>313</v>
+        <v>452</v>
       </c>
       <c r="D56" s="3">
-        <v>40</v>
-      </c>
-      <c r="E56" s="3">
-        <v>149</v>
+        <v>41</v>
+      </c>
+      <c r="E56" s="4">
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>3728</v>
+        <v>3374</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C57" s="3">
-        <v>313</v>
+        <v>288</v>
       </c>
       <c r="D57" s="3">
-        <v>40</v>
-      </c>
-      <c r="E57" s="3">
-        <v>149</v>
+        <v>39</v>
+      </c>
+      <c r="E57" s="4">
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>5479</v>
+        <v>3375</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C58" s="3">
-        <v>359</v>
+        <v>256</v>
       </c>
       <c r="D58" s="3">
-        <v>42</v>
-      </c>
-      <c r="E58" s="3">
-        <v>183</v>
+        <v>39</v>
+      </c>
+      <c r="E58" s="4">
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>5480</v>
+        <v>3376</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C59" s="3">
-        <v>26</v>
+        <v>246</v>
       </c>
       <c r="D59" s="3">
-        <v>26</v>
-      </c>
-      <c r="E59" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="E59" s="4">
+        <v>132</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>5481</v>
+        <v>3377</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C60" s="3">
-        <v>34</v>
+        <v>256</v>
       </c>
       <c r="D60" s="3">
-        <v>34</v>
-      </c>
-      <c r="E60" s="3">
-        <v>131</v>
+        <v>39</v>
+      </c>
+      <c r="E60" s="4">
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>5482</v>
+        <v>3378</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C61" s="3">
-        <v>34</v>
+        <v>245</v>
       </c>
       <c r="D61" s="3">
-        <v>34</v>
-      </c>
-      <c r="E61" s="3">
-        <v>131</v>
+        <v>37</v>
+      </c>
+      <c r="E61" s="4">
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>5483</v>
+        <v>3379</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C62" s="3">
-        <v>38</v>
+        <v>245</v>
       </c>
       <c r="D62" s="3">
-        <v>38</v>
-      </c>
-      <c r="E62" s="3">
-        <v>159</v>
+        <v>37</v>
+      </c>
+      <c r="E62" s="4">
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>5484</v>
+        <v>3380</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C63" s="3">
-        <v>38</v>
+        <v>245</v>
       </c>
       <c r="D63" s="3">
-        <v>38</v>
-      </c>
-      <c r="E63" s="3">
-        <v>159</v>
+        <v>37</v>
+      </c>
+      <c r="E63" s="4">
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>5485</v>
+        <v>3718</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C64" s="3">
-        <v>303</v>
+        <v>329</v>
       </c>
       <c r="D64" s="3">
-        <v>37</v>
-      </c>
-      <c r="E64" s="3">
-        <v>144</v>
+        <v>35</v>
+      </c>
+      <c r="E64" s="4">
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>5486</v>
+        <v>3719</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C65" s="3">
-        <v>303</v>
+        <v>329</v>
       </c>
       <c r="D65" s="3">
-        <v>37</v>
-      </c>
-      <c r="E65" s="3">
-        <v>145</v>
+        <v>35</v>
+      </c>
+      <c r="E65" s="4">
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>5487</v>
+        <v>3720</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C66" s="3">
-        <v>303</v>
+        <v>329</v>
       </c>
       <c r="D66" s="3">
-        <v>37</v>
-      </c>
-      <c r="E66" s="3">
-        <v>144</v>
+        <v>35</v>
+      </c>
+      <c r="E66" s="4">
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>5682</v>
+        <v>3721</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C67" s="3">
-        <v>31</v>
+        <v>329</v>
       </c>
       <c r="D67" s="3">
-        <v>31</v>
-      </c>
-      <c r="E67" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E67" s="4">
+        <v>112</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>5683</v>
+        <v>3722</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C68" s="3">
-        <v>359</v>
+        <v>330</v>
       </c>
       <c r="D68" s="3">
-        <v>36</v>
-      </c>
-      <c r="E68" s="3">
-        <v>130</v>
+        <v>35</v>
+      </c>
+      <c r="E68" s="4">
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>5684</v>
+        <v>3723</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C69" s="3">
-        <v>378</v>
+        <v>330</v>
       </c>
       <c r="D69" s="3">
-        <v>38</v>
-      </c>
-      <c r="E69" s="3">
-        <v>164</v>
+        <v>35</v>
+      </c>
+      <c r="E69" s="4">
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>6195</v>
+        <v>3724</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C70" s="3">
-        <v>31</v>
+        <v>313</v>
       </c>
       <c r="D70" s="3">
-        <v>31</v>
-      </c>
-      <c r="E70" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="E70" s="4">
+        <v>149</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>6196</v>
+        <v>3725</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C71" s="3">
-        <v>76</v>
+        <v>313</v>
       </c>
       <c r="D71" s="3">
-        <v>38</v>
-      </c>
-      <c r="E71" s="3">
-        <v>114</v>
+        <v>40</v>
+      </c>
+      <c r="E71" s="4">
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>6294</v>
+        <v>3726</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C72" s="3">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="D72" s="3">
-        <v>39</v>
-      </c>
-      <c r="E72" s="3">
-        <v>155</v>
+        <v>40</v>
+      </c>
+      <c r="E72" s="4">
+        <v>149</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>6295</v>
+        <v>3727</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C73" s="3">
-        <v>30</v>
+        <v>313</v>
       </c>
       <c r="D73" s="3">
-        <v>30</v>
-      </c>
-      <c r="E73" s="3">
-        <v>159</v>
+        <v>40</v>
+      </c>
+      <c r="E73" s="4">
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>6296</v>
+        <v>3728</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C74" s="3">
-        <v>34</v>
+        <v>313</v>
       </c>
       <c r="D74" s="3">
-        <v>34</v>
-      </c>
-      <c r="E74" s="3">
-        <v>158</v>
+        <v>40</v>
+      </c>
+      <c r="E74" s="4">
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>6721</v>
+        <v>5479</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C75" s="3">
-        <v>37</v>
+        <v>359</v>
       </c>
       <c r="D75" s="3">
-        <v>37</v>
-      </c>
-      <c r="E75" s="3">
-        <v>113</v>
+        <v>42</v>
+      </c>
+      <c r="E75" s="4">
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>6722</v>
+        <v>5480</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C76" s="3">
-        <v>318</v>
+        <v>26</v>
       </c>
       <c r="D76" s="3">
-        <v>38</v>
-      </c>
-      <c r="E76" s="3">
-        <v>117</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E76" s="5"/>
     </row>
     <row r="77" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>6723</v>
+        <v>5481</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C77" s="3">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D77" s="3">
-        <v>37</v>
-      </c>
-      <c r="E77" s="3">
-        <v>113</v>
+        <v>34</v>
+      </c>
+      <c r="E77" s="4">
+        <v>131</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>6724</v>
+        <v>5482</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C78" s="3">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D78" s="3">
-        <v>37</v>
-      </c>
-      <c r="E78" s="3">
-        <v>113</v>
+        <v>34</v>
+      </c>
+      <c r="E78" s="4">
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>6787</v>
+        <v>5483</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C79" s="3">
-        <v>300</v>
+        <v>38</v>
       </c>
       <c r="D79" s="3">
         <v>38</v>
       </c>
-      <c r="E79" s="3">
-        <v>138</v>
+      <c r="E79" s="4">
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>6788</v>
+        <v>5484</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C80" s="3">
-        <v>300</v>
+        <v>38</v>
       </c>
       <c r="D80" s="3">
         <v>38</v>
       </c>
-      <c r="E80" s="3">
-        <v>138</v>
+      <c r="E80" s="4">
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>6789</v>
+        <v>5485</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C81" s="3">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D81" s="3">
-        <v>38</v>
-      </c>
-      <c r="E81" s="3">
-        <v>168</v>
+        <v>37</v>
+      </c>
+      <c r="E81" s="4">
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>6896</v>
+        <v>5486</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C82" s="3">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="D82" s="3">
-        <v>40</v>
-      </c>
-      <c r="E82" s="3">
-        <v>157</v>
+        <v>37</v>
+      </c>
+      <c r="E82" s="4">
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>6897</v>
+        <v>5487</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C83" s="3">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="D83" s="3">
-        <v>39</v>
-      </c>
-      <c r="E83" s="3">
-        <v>156</v>
+        <v>37</v>
+      </c>
+      <c r="E83" s="4">
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>7276</v>
+        <v>5682</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C84" s="3">
-        <v>379</v>
+        <v>31</v>
       </c>
       <c r="D84" s="3">
-        <v>40</v>
-      </c>
-      <c r="E84" s="3">
-        <v>151</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E84" s="5"/>
     </row>
     <row r="85" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>7277</v>
+        <v>5683</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C85" s="3">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="D85" s="3">
-        <v>40</v>
-      </c>
-      <c r="E85" s="3">
-        <v>119</v>
+        <v>36</v>
+      </c>
+      <c r="E85" s="4">
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>7278</v>
+        <v>5684</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C86" s="3">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="D86" s="3">
-        <v>40</v>
-      </c>
-      <c r="E86" s="3">
-        <v>177</v>
+        <v>38</v>
+      </c>
+      <c r="E86" s="4">
+        <v>164</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>7447</v>
+        <v>6195</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C87" s="3">
-        <v>382</v>
+        <v>31</v>
       </c>
       <c r="D87" s="3">
-        <v>36</v>
-      </c>
-      <c r="E87" s="3">
-        <v>126</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E87" s="5"/>
     </row>
     <row r="88" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>7448</v>
+        <v>6196</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C88" s="3">
-        <v>263</v>
+        <v>76</v>
       </c>
       <c r="D88" s="3">
-        <v>35</v>
-      </c>
-      <c r="E88" s="3">
-        <v>199</v>
+        <v>38</v>
+      </c>
+      <c r="E88" s="4">
+        <v>114</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>7449</v>
+        <v>6294</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C89" s="3">
-        <v>372</v>
+        <v>325</v>
       </c>
       <c r="D89" s="3">
-        <v>36</v>
-      </c>
-      <c r="E89" s="3">
-        <v>116</v>
+        <v>39</v>
+      </c>
+      <c r="E89" s="4">
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>7450</v>
+        <v>6295</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C90" s="3">
-        <v>263</v>
+        <v>30</v>
       </c>
       <c r="D90" s="3">
-        <v>36</v>
-      </c>
-      <c r="E90" s="3">
-        <v>186</v>
+        <v>30</v>
+      </c>
+      <c r="E90" s="4">
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>7634</v>
+        <v>6296</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C91" s="3">
-        <v>296</v>
+        <v>34</v>
       </c>
       <c r="D91" s="3">
         <v>34</v>
       </c>
-      <c r="E91" s="3">
-        <v>126</v>
+      <c r="E91" s="4">
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>7635</v>
+        <v>6721</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="C92" s="3">
-        <v>291</v>
+        <v>37</v>
       </c>
       <c r="D92" s="3">
-        <v>34</v>
-      </c>
-      <c r="E92" s="3">
-        <v>121</v>
+        <v>37</v>
+      </c>
+      <c r="E92" s="4">
+        <v>113</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>7636</v>
+        <v>6722</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C93" s="3">
-        <v>200</v>
+        <v>318</v>
       </c>
       <c r="D93" s="3">
         <v>38</v>
       </c>
-      <c r="E93" s="3">
-        <v>135</v>
+      <c r="E93" s="4">
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>7637</v>
+        <v>6723</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C94" s="3">
-        <v>292</v>
+        <v>37</v>
       </c>
       <c r="D94" s="3">
-        <v>76</v>
-      </c>
-      <c r="E94" s="3">
-        <v>153</v>
+        <v>37</v>
+      </c>
+      <c r="E94" s="4">
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>8749</v>
+        <v>6724</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="C95" s="3">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D95" s="3">
-        <v>32</v>
-      </c>
-      <c r="E95" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E95" s="4">
+        <v>113</v>
+      </c>
     </row>
     <row r="96" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>8750</v>
+        <v>6787</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="C96" s="3">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="D96" s="3">
-        <v>37</v>
-      </c>
-      <c r="E96" s="3">
-        <v>108</v>
+        <v>38</v>
+      </c>
+      <c r="E96" s="4">
+        <v>138</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>8751</v>
+        <v>6788</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C97" s="3">
-        <v>32</v>
+        <v>300</v>
       </c>
       <c r="D97" s="3">
-        <v>32</v>
-      </c>
-      <c r="E97" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="E97" s="4">
+        <v>138</v>
+      </c>
     </row>
     <row r="98" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>8752</v>
+        <v>6789</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C98" s="3">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D98" s="3">
-        <v>40</v>
-      </c>
-      <c r="E98" s="3">
-        <v>157</v>
+        <v>38</v>
+      </c>
+      <c r="E98" s="4">
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>8753</v>
+        <v>6896</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C99" s="3">
-        <v>223</v>
+        <v>319</v>
       </c>
       <c r="D99" s="3">
         <v>40</v>
       </c>
-      <c r="E99" s="3">
-        <v>150</v>
+      <c r="E99" s="4">
+        <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>9774</v>
+        <v>6897</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C100" s="3">
-        <v>34</v>
+        <v>319</v>
       </c>
       <c r="D100" s="3">
-        <v>34</v>
-      </c>
-      <c r="E100" s="3">
-        <v>210</v>
+        <v>39</v>
+      </c>
+      <c r="E100" s="4">
+        <v>156</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>9775</v>
+        <v>7276</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C101" s="3">
-        <v>33</v>
+        <v>379</v>
       </c>
       <c r="D101" s="3">
-        <v>33</v>
-      </c>
-      <c r="E101" s="3">
-        <v>194</v>
+        <v>40</v>
+      </c>
+      <c r="E101" s="4">
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>9776</v>
+        <v>7277</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C102" s="3">
-        <v>31</v>
+        <v>353</v>
       </c>
       <c r="D102" s="3">
-        <v>31</v>
-      </c>
-      <c r="E102" s="3">
-        <v>160</v>
+        <v>40</v>
+      </c>
+      <c r="E102" s="4">
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>9777</v>
+        <v>7278</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C103" s="3">
-        <v>375</v>
+        <v>391</v>
       </c>
       <c r="D103" s="3">
-        <v>37</v>
-      </c>
-      <c r="E103" s="3">
-        <v>154</v>
+        <v>40</v>
+      </c>
+      <c r="E103" s="4">
+        <v>177</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
+        <v>7447</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C104" s="3">
+        <v>382</v>
+      </c>
+      <c r="D104" s="3">
+        <v>36</v>
+      </c>
+      <c r="E104" s="4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>7448</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C105" s="3">
+        <v>263</v>
+      </c>
+      <c r="D105" s="3">
+        <v>35</v>
+      </c>
+      <c r="E105" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>7449</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C106" s="3">
+        <v>372</v>
+      </c>
+      <c r="D106" s="3">
+        <v>36</v>
+      </c>
+      <c r="E106" s="4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>7450</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C107" s="3">
+        <v>263</v>
+      </c>
+      <c r="D107" s="3">
+        <v>36</v>
+      </c>
+      <c r="E107" s="4">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>7634</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C108" s="3">
+        <v>296</v>
+      </c>
+      <c r="D108" s="3">
+        <v>34</v>
+      </c>
+      <c r="E108" s="4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>7635</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C109" s="3">
+        <v>291</v>
+      </c>
+      <c r="D109" s="3">
+        <v>34</v>
+      </c>
+      <c r="E109" s="4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>7636</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C110" s="3">
+        <v>200</v>
+      </c>
+      <c r="D110" s="3">
+        <v>38</v>
+      </c>
+      <c r="E110" s="4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>7637</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C111" s="3">
+        <v>292</v>
+      </c>
+      <c r="D111" s="3">
+        <v>76</v>
+      </c>
+      <c r="E111" s="4">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>8749</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C112" s="3">
+        <v>32</v>
+      </c>
+      <c r="D112" s="3">
+        <v>32</v>
+      </c>
+      <c r="E112" s="5"/>
+    </row>
+    <row r="113" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>8750</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C113" s="3">
+        <v>282</v>
+      </c>
+      <c r="D113" s="3">
+        <v>37</v>
+      </c>
+      <c r="E113" s="4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>8751</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C114" s="3">
+        <v>32</v>
+      </c>
+      <c r="D114" s="3">
+        <v>32</v>
+      </c>
+      <c r="E114" s="5"/>
+    </row>
+    <row r="115" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>8752</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C115" s="3">
+        <v>297</v>
+      </c>
+      <c r="D115" s="3">
+        <v>40</v>
+      </c>
+      <c r="E115" s="4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>8753</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C116" s="3">
+        <v>223</v>
+      </c>
+      <c r="D116" s="3">
+        <v>40</v>
+      </c>
+      <c r="E116" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>9774</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C117" s="3">
+        <v>34</v>
+      </c>
+      <c r="D117" s="3">
+        <v>34</v>
+      </c>
+      <c r="E117" s="4">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>9775</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C118" s="3">
+        <v>33</v>
+      </c>
+      <c r="D118" s="3">
+        <v>33</v>
+      </c>
+      <c r="E118" s="4">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>9776</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C119" s="3">
+        <v>31</v>
+      </c>
+      <c r="D119" s="3">
+        <v>31</v>
+      </c>
+      <c r="E119" s="4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>9777</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C120" s="3">
+        <v>375</v>
+      </c>
+      <c r="D120" s="3">
+        <v>37</v>
+      </c>
+      <c r="E120" s="4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
         <v>9778</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C104" s="3">
+      <c r="C121" s="3">
         <v>459</v>
       </c>
-      <c r="D104" s="3">
+      <c r="D121" s="3">
         <v>37</v>
       </c>
-      <c r="E104" s="3">
+      <c r="E121" s="4">
         <v>175</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>